<commit_message>
Feedback on first version of the production Definition
</commit_message>
<xml_diff>
--- a/Zacher/Deliverables Tracking.xlsx
+++ b/Zacher/Deliverables Tracking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="29780" yWindow="180" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Professionalism" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>Deliverables Tracking</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>End of Day</t>
+  </si>
+  <si>
+    <t>Interface list</t>
   </si>
 </sst>
 </file>
@@ -223,8 +226,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="237">
+  <cellStyleXfs count="239">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -512,7 +517,7 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="237">
+  <cellStyles count="239">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -631,6 +636,7 @@
     <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -749,6 +755,7 @@
     <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1238,10 +1245,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1377,71 +1384,80 @@
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="13"/>
-      <c r="E10"/>
+      <c r="B10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="D10" s="17">
+        <v>42872</v>
+      </c>
+      <c r="E10" s="17">
+        <v>42874</v>
+      </c>
+      <c r="F10" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C11" s="13"/>
       <c r="E11"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" s="13"/>
       <c r="E12"/>
     </row>
     <row r="13" spans="1:12">
+      <c r="A13" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="C13" s="13"/>
       <c r="E13"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="5"/>
       <c r="C14" s="13"/>
       <c r="E14"/>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="13"/>
+      <c r="E15"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="12"/>
-      <c r="E15"/>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="13"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="12"/>
       <c r="E16"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C17" s="13"/>
       <c r="E17"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="2"/>
+      <c r="A18" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="C18" s="13"/>
       <c r="E18"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="13"/>
@@ -1449,101 +1465,109 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="13"/>
       <c r="E20"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="6"/>
+      <c r="A21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="2"/>
       <c r="C21" s="13"/>
       <c r="E21"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="6"/>
+      <c r="A22" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="B22" s="6"/>
       <c r="C22" s="13"/>
       <c r="E22"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="13"/>
+      <c r="E23"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="12"/>
-      <c r="E23"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="B24" s="6"/>
       <c r="C24" s="12"/>
       <c r="E24"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C25" s="12"/>
       <c r="E25"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C26" s="12"/>
       <c r="E26"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C27" s="12"/>
       <c r="E27"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" s="5"/>
+      <c r="A28" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="C28" s="12"/>
       <c r="E28"/>
     </row>
     <row r="29" spans="1:5">
+      <c r="A29" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="5"/>
       <c r="C29" s="12"/>
       <c r="E29"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" s="6"/>
       <c r="C30" s="12"/>
       <c r="E30"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="A31" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="6"/>
       <c r="C31" s="12"/>
       <c r="E31"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C32" s="12"/>
       <c r="E32"/>
     </row>
-    <row r="33" spans="3:3">
+    <row r="33" spans="1:5">
+      <c r="A33" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="C33" s="12"/>
-    </row>
-    <row r="34" spans="3:3">
+      <c r="E33"/>
+    </row>
+    <row r="34" spans="1:5">
       <c r="C34" s="12"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="C35" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Updated Feedback, Architectural Deliverables, and Task Enumeration
</commit_message>
<xml_diff>
--- a/Zacher/Deliverables Tracking.xlsx
+++ b/Zacher/Deliverables Tracking.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3540" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Professionalism" sheetId="2" r:id="rId1"/>
     <sheet name="Hardware Development Process" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
   <si>
     <t>Deliverables Tracking</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>Interface list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fill in Task Enumeration for Product Definition </t>
   </si>
 </sst>
 </file>
@@ -226,8 +229,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="239">
+  <cellStyleXfs count="249">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -517,7 +530,7 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="239">
+  <cellStyles count="249">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -637,6 +650,11 @@
     <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -756,6 +774,11 @@
     <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1245,10 +1268,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1404,68 +1427,107 @@
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="E11"/>
+      <c r="C11" s="13">
+        <v>2</v>
+      </c>
+      <c r="D11" s="17">
+        <v>42871</v>
+      </c>
+      <c r="E11" s="17">
+        <v>42878</v>
+      </c>
+      <c r="F11" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="E12"/>
+      <c r="C12" s="13">
+        <v>2</v>
+      </c>
+      <c r="D12" s="17">
+        <v>42871</v>
+      </c>
+      <c r="E12" s="17">
+        <v>42878</v>
+      </c>
+      <c r="F12" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="E13"/>
+      <c r="C13" s="13">
+        <v>2</v>
+      </c>
+      <c r="D13" s="17">
+        <v>42871</v>
+      </c>
+      <c r="E13" s="17">
+        <v>42878</v>
+      </c>
+      <c r="F13" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="C14" s="13"/>
-      <c r="E14"/>
+      <c r="A14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="13">
+        <v>2</v>
+      </c>
+      <c r="D14" s="17">
+        <v>42871</v>
+      </c>
+      <c r="E14" s="17">
+        <v>42878</v>
+      </c>
+      <c r="F14" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="5"/>
       <c r="C15" s="13"/>
       <c r="E15"/>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="13"/>
+      <c r="E16"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="12"/>
-      <c r="E16"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="13"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="12"/>
       <c r="E17"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C18" s="13"/>
       <c r="E18"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="2"/>
+      <c r="A19" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="C19" s="13"/>
       <c r="E19"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="13"/>
@@ -1473,101 +1535,109 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="13"/>
       <c r="E21"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="6"/>
+      <c r="A22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="2"/>
       <c r="C22" s="13"/>
       <c r="E22"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="6"/>
+      <c r="A23" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="B23" s="6"/>
       <c r="C23" s="13"/>
       <c r="E23"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="13"/>
+      <c r="E24"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="12"/>
-      <c r="E24"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="B25" s="6"/>
       <c r="C25" s="12"/>
       <c r="E25"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C26" s="12"/>
       <c r="E26"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C27" s="12"/>
       <c r="E27"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C28" s="12"/>
       <c r="E28"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" s="5"/>
+      <c r="A29" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="C29" s="12"/>
       <c r="E29"/>
     </row>
     <row r="30" spans="1:5">
+      <c r="A30" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" s="5"/>
       <c r="C30" s="12"/>
       <c r="E30"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B31" s="6"/>
       <c r="C31" s="12"/>
       <c r="E31"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="A32" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" s="6"/>
       <c r="C32" s="12"/>
       <c r="E32"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C33" s="12"/>
       <c r="E33"/>
     </row>
     <row r="34" spans="1:5">
+      <c r="A34" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="C34" s="12"/>
+      <c r="E34"/>
     </row>
     <row r="35" spans="1:5">
       <c r="C35" s="12"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="C36" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Added Realization deliverables and architecture task enumeration
</commit_message>
<xml_diff>
--- a/Zacher/Deliverables Tracking.xlsx
+++ b/Zacher/Deliverables Tracking.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zache_000\Documents\GitHub\Independent\Zacher\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="0" windowWidth="25605" windowHeight="16065" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3080" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Professionalism" sheetId="2" r:id="rId1"/>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
   <si>
     <t>Deliverables Tracking</t>
   </si>
@@ -154,6 +149,9 @@
   </si>
   <si>
     <t xml:space="preserve">Fill in Task Enumeration for Product Definition </t>
+  </si>
+  <si>
+    <t>Make update to Architecture</t>
   </si>
 </sst>
 </file>
@@ -233,8 +231,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="249">
+  <cellStyleXfs count="261">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -534,7 +544,7 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="249">
+  <cellStyles count="261">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -659,6 +669,12 @@
     <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -783,6 +799,12 @@
     <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1194,22 +1216,22 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="16">
       <c r="A1" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="9"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="18">
       <c r="A2" s="8" t="s">
         <v>19</v>
       </c>
@@ -1218,19 +1240,19 @@
       </c>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="18">
       <c r="A3" s="8"/>
       <c r="B3" s="10"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="16">
       <c r="A4" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="9"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="1" customFormat="1" ht="30">
       <c r="A5" s="7" t="s">
         <v>0</v>
       </c>
@@ -1253,17 +1275,17 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="32">
       <c r="A6" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="16">
       <c r="A7" s="15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="32">
       <c r="A8" s="15" t="s">
         <v>33</v>
       </c>
@@ -1280,34 +1302,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="44.5" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.5" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.125" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="16">
       <c r="A1" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="9"/>
     </row>
-    <row r="2" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="18">
       <c r="A2" s="8" t="s">
         <v>19</v>
       </c>
@@ -1316,19 +1338,19 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="18">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="10"/>
     </row>
-    <row r="4" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="16">
       <c r="A4" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="9"/>
     </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="1" customFormat="1" ht="30">
       <c r="A5" s="7" t="s">
         <v>0</v>
       </c>
@@ -1360,7 +1382,7 @@
       <c r="K5"/>
       <c r="L5"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" s="3" t="s">
         <v>37</v>
       </c>
@@ -1377,14 +1399,14 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="12"/>
       <c r="E7"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="B8" s="3" t="s">
         <v>38</v>
       </c>
@@ -1401,7 +1423,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="B9" s="3" t="s">
         <v>39</v>
       </c>
@@ -1418,7 +1440,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="B10" s="3" t="s">
         <v>41</v>
       </c>
@@ -1435,7 +1457,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
@@ -1452,7 +1474,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
@@ -1469,7 +1491,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13" s="3" t="s">
         <v>5</v>
       </c>
@@ -1486,7 +1508,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14" s="3" t="s">
         <v>42</v>
       </c>
@@ -1503,11 +1525,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="C15" s="13"/>
       <c r="E15"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16" s="5" t="s">
         <v>34</v>
       </c>
@@ -1515,141 +1537,209 @@
       <c r="C16" s="13"/>
       <c r="E16"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="13">
+        <v>3</v>
+      </c>
+      <c r="D17" s="17">
+        <v>42879</v>
+      </c>
+      <c r="E17" s="17">
+        <v>42885</v>
+      </c>
+      <c r="F17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="12"/>
-      <c r="E17"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="B18" s="5"/>
+      <c r="C18" s="12">
+        <v>3</v>
+      </c>
+      <c r="D18" s="17">
+        <v>42879</v>
+      </c>
+      <c r="E18" s="17">
+        <v>42912</v>
+      </c>
+      <c r="F18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="E18"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="C19" s="13">
+        <v>3</v>
+      </c>
+      <c r="D19" s="17">
+        <v>42879</v>
+      </c>
+      <c r="E19" s="17">
+        <v>42912</v>
+      </c>
+      <c r="F19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="E19"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="C20" s="13">
+        <v>3</v>
+      </c>
+      <c r="D20" s="17">
+        <v>42879</v>
+      </c>
+      <c r="E20" s="17">
+        <v>42912</v>
+      </c>
+      <c r="F20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="13"/>
-      <c r="E20"/>
-    </row>
-    <row r="21" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="B21" s="2"/>
+      <c r="C21" s="13">
+        <v>3</v>
+      </c>
+      <c r="D21" s="17">
+        <v>42879</v>
+      </c>
+      <c r="E21" s="17">
+        <v>42912</v>
+      </c>
+      <c r="F21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="13"/>
-      <c r="E21"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="B22" s="2"/>
+      <c r="C22" s="13">
+        <v>3</v>
+      </c>
+      <c r="D22" s="17">
+        <v>42879</v>
+      </c>
+      <c r="E22" s="17">
+        <v>42912</v>
+      </c>
+      <c r="F22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="13"/>
-      <c r="E22"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="6"/>
+      <c r="B23" s="2"/>
       <c r="C23" s="13"/>
       <c r="E23"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
+    <row r="24" spans="1:6">
+      <c r="A24" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="B24" s="6"/>
       <c r="C24" s="13"/>
       <c r="E24"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+    <row r="25" spans="1:6">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="13"/>
+      <c r="E25"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="12"/>
-      <c r="E25"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="B26" s="6"/>
       <c r="C26" s="12"/>
       <c r="E26"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C27" s="12"/>
       <c r="E27"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C28" s="12"/>
       <c r="E28"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C29" s="12"/>
       <c r="E29"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" s="5"/>
+    <row r="30" spans="1:6">
+      <c r="A30" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="C30" s="12"/>
       <c r="E30"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
+      <c r="A31" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="5"/>
       <c r="C31" s="12"/>
       <c r="E31"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" s="6"/>
+    <row r="32" spans="1:6">
       <c r="C32" s="12"/>
       <c r="E32"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>23</v>
-      </c>
+    <row r="33" spans="1:5">
+      <c r="A33" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="6"/>
       <c r="C33" s="12"/>
       <c r="E33"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C34" s="12"/>
       <c r="E34"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
+      <c r="A35" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="C35" s="12"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E35"/>
+    </row>
+    <row r="36" spans="1:5">
       <c r="C36" s="12"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="C37" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Update independent tracking documents
</commit_message>
<xml_diff>
--- a/Zacher/Deliverables Tracking.xlsx
+++ b/Zacher/Deliverables Tracking.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Professionalism" sheetId="2" r:id="rId1"/>
     <sheet name="Hardware Development Process" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="152511" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1310,7 +1310,7 @@
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated status of deliverables
</commit_message>
<xml_diff>
--- a/Zacher/Deliverables Tracking.xlsx
+++ b/Zacher/Deliverables Tracking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-34760" yWindow="4660" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Professionalism" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
   <si>
     <t>Deliverables Tracking</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Eagle Library</t>
   </si>
   <si>
-    <t>Feature and Behavior Acceptance criteria</t>
-  </si>
-  <si>
     <t>Board Fab and Build</t>
   </si>
   <si>
@@ -79,9 +76,6 @@
     <t xml:space="preserve">Session </t>
   </si>
   <si>
-    <t>Estimate Task Hours</t>
-  </si>
-  <si>
     <t>Enter Hours Spent</t>
   </si>
   <si>
@@ -103,21 +97,9 @@
     <t>Review, Release, Version Control Lists</t>
   </si>
   <si>
-    <t>Estimated Hours</t>
-  </si>
-  <si>
-    <t>Actual Hours</t>
-  </si>
-  <si>
     <t>Choose a task list format</t>
   </si>
   <si>
-    <t>Estimate Architecture Task Hours</t>
-  </si>
-  <si>
-    <t>Zacher Tiburzi</t>
-  </si>
-  <si>
     <t xml:space="preserve">Independent </t>
   </si>
   <si>
@@ -158,6 +140,15 @@
   </si>
   <si>
     <t xml:space="preserve">Eagle Layout Cut Ready </t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t>End of Class</t>
   </si>
 </sst>
 </file>
@@ -225,12 +216,30 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -242,7 +251,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="287">
+  <cellStyleXfs count="311">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -530,8 +539,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -583,8 +616,11 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="287">
+  <cellStyles count="311">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -728,6 +764,18 @@
     <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -871,6 +919,18 @@
     <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1292,17 +1352,17 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16">
       <c r="A1" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="9"/>
       <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:6" ht="18">
       <c r="A2" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D2" s="3"/>
     </row>
@@ -1313,7 +1373,7 @@
     </row>
     <row r="4" spans="1:6" ht="16">
       <c r="A4" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" s="9"/>
       <c r="D4" s="3"/>
@@ -1323,16 +1383,16 @@
         <v>0</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>2</v>
@@ -1340,7 +1400,7 @@
     </row>
     <row r="6" spans="1:6" ht="32">
       <c r="A6" s="17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1352,12 +1412,12 @@
         <v>42935</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16">
       <c r="A7" s="17" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1369,7 +1429,7 @@
         <v>42935</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16">
@@ -1388,92 +1448,87 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="44.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16">
+    <row r="1" spans="1:10" ht="16">
       <c r="A1" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="9"/>
     </row>
-    <row r="2" spans="1:12" ht="18">
+    <row r="2" spans="1:10" ht="18">
       <c r="A2" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="15" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="18">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="18">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="10"/>
     </row>
-    <row r="4" spans="1:12" ht="16">
+    <row r="4" spans="1:10" ht="16">
       <c r="A4" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="9"/>
     </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" ht="30">
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="30">
       <c r="A5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="I5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K5"/>
-      <c r="L5"/>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="C6" s="12">
         <v>1</v>
@@ -1485,19 +1540,20 @@
         <v>42871</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+        <v>30</v>
+      </c>
+      <c r="G6" s="20"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="12"/>
       <c r="E7"/>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:10">
       <c r="B8" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C8" s="12">
         <v>1</v>
@@ -1509,12 +1565,13 @@
         <v>42871</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>30</v>
+      </c>
+      <c r="G8" s="20"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="B9" s="3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C9" s="12">
         <v>1</v>
@@ -1526,12 +1583,13 @@
         <v>42871</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>30</v>
+      </c>
+      <c r="G9" s="20"/>
+    </row>
+    <row r="10" spans="1:10">
       <c r="B10" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C10" s="12">
         <v>1.5</v>
@@ -1543,10 +1601,11 @@
         <v>42874</v>
       </c>
       <c r="F10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>30</v>
+      </c>
+      <c r="G10" s="20"/>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
@@ -1560,10 +1619,10 @@
         <v>42878</v>
       </c>
       <c r="F11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
@@ -1577,10 +1636,11 @@
         <v>42878</v>
       </c>
       <c r="F12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+        <v>30</v>
+      </c>
+      <c r="G12" s="21"/>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="3" t="s">
         <v>5</v>
       </c>
@@ -1594,12 +1654,13 @@
         <v>42878</v>
       </c>
       <c r="F13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+        <v>30</v>
+      </c>
+      <c r="G13" s="19"/>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C14" s="13">
         <v>2</v>
@@ -1611,26 +1672,37 @@
         <v>42878</v>
       </c>
       <c r="F14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>30</v>
+      </c>
+      <c r="G14" s="19"/>
+    </row>
+    <row r="15" spans="1:10">
       <c r="C15" s="13"/>
       <c r="E15"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:10">
       <c r="A16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="13">
+        <v>3</v>
+      </c>
+      <c r="D16" s="16">
+        <v>42879</v>
+      </c>
+      <c r="E16" s="16">
+        <v>42885</v>
+      </c>
+      <c r="F16" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="13"/>
-      <c r="E16"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="5"/>
+      <c r="G16" s="19"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="C17" s="13">
         <v>3</v>
       </c>
@@ -1638,34 +1710,36 @@
         <v>42879</v>
       </c>
       <c r="E17" s="16">
-        <v>42885</v>
+        <v>42912</v>
       </c>
       <c r="F17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="12">
+        <v>30</v>
+      </c>
+      <c r="G17" s="19"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="13">
         <v>3</v>
       </c>
       <c r="D18" s="16">
         <v>42879</v>
       </c>
       <c r="E18" s="16">
-        <v>42912</v>
+        <v>42924</v>
       </c>
       <c r="F18" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="G18" s="20"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="2"/>
       <c r="C19" s="13">
         <v>3</v>
       </c>
@@ -1673,204 +1747,128 @@
         <v>42879</v>
       </c>
       <c r="E19" s="16">
-        <v>42912</v>
+        <v>42928</v>
       </c>
       <c r="F19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="13">
-        <v>3</v>
-      </c>
-      <c r="D20" s="16">
-        <v>42879</v>
-      </c>
-      <c r="E20" s="16">
-        <v>42924</v>
-      </c>
-      <c r="F20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G19" s="20"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="13">
-        <v>3</v>
-      </c>
-      <c r="D21" s="16">
-        <v>42879</v>
-      </c>
-      <c r="E21" s="16">
-        <v>42928</v>
+        <v>5</v>
+      </c>
+      <c r="D21" s="18">
+        <v>42924</v>
+      </c>
+      <c r="E21" s="18">
+        <v>42938</v>
       </c>
       <c r="F21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="13">
-        <v>5</v>
-      </c>
-      <c r="D23" s="18">
-        <v>42924</v>
-      </c>
-      <c r="E23" s="18">
-        <v>42938</v>
+        <v>36</v>
+      </c>
+      <c r="G21" s="19"/>
+      <c r="I21" s="16">
+        <v>42940</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="12">
+        <v>6</v>
+      </c>
+      <c r="E23" s="16">
+        <v>42952</v>
       </c>
       <c r="F23" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="13"/>
+      <c r="G23" s="21"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="12">
+        <v>6</v>
+      </c>
+      <c r="E24" s="16">
+        <v>42952</v>
+      </c>
+      <c r="F24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="21"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="12"/>
+      <c r="E25"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="12"/>
+      <c r="E26"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="C27" s="12"/>
       <c r="E27"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:9">
       <c r="A28" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B28" s="6"/>
-      <c r="C28" s="13"/>
+      <c r="C28" s="12"/>
       <c r="E28"/>
     </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="13"/>
+    <row r="29" spans="1:9">
+      <c r="A29" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="12"/>
       <c r="E29"/>
     </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B30" s="6"/>
+    <row r="30" spans="1:9">
+      <c r="A30" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="C30" s="12"/>
       <c r="E30"/>
     </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="3" t="s">
-        <v>14</v>
-      </c>
+    <row r="31" spans="1:9">
       <c r="C31" s="12"/>
-      <c r="E31"/>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="3" t="s">
-        <v>11</v>
-      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="C32" s="12"/>
-      <c r="E32"/>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C33" s="12"/>
-      <c r="E33"/>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" s="12"/>
-      <c r="E34"/>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="12"/>
-      <c r="E35"/>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="C36" s="12"/>
-      <c r="E36"/>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="12"/>
-      <c r="E37"/>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C38" s="12"/>
-      <c r="E38"/>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C39" s="12"/>
-      <c r="E39"/>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="C40" s="12"/>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="C41" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>